<commit_message>
created : from dates and to dates in certificate
</commit_message>
<xml_diff>
--- a/Contact Information.xlsx
+++ b/Contact Information.xlsx
@@ -620,7 +620,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.630000000000001" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="12" width="18.879999999999999"/>
+    <col customWidth="1" min="1" max="1" width="19.140625"/>
+    <col customWidth="1" min="2" max="2" width="18.879999999999999"/>
+    <col customWidth="1" min="3" max="3" width="28.7109375"/>
+    <col customWidth="1" min="4" max="12" width="18.879999999999999"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>